<commit_message>
updated spreadsheet with missing URLs
</commit_message>
<xml_diff>
--- a/assets/files/redirect.xlsx
+++ b/assets/files/redirect.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
   <si>
     <t>Table 1</t>
   </si>
@@ -471,7 +471,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -479,7 +479,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/resources/awardees/</t>
@@ -504,7 +504,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -512,7 +512,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/resources/awardees/ambassador/</t>
@@ -537,7 +537,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -545,7 +545,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/assets/files/awardees/NSF_SBIR_Abassador_Toolkit.pdf</t>
@@ -570,7 +570,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -578,7 +578,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/resources/awardees/reporting/phase-1/</t>
@@ -603,7 +603,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -611,7 +611,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/resources/awardees/researchexp/</t>
@@ -643,7 +643,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov/assets/files/awardees/RET_Flyer.pdf</t>
@@ -667,7 +667,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov/assets/files/awardees/RAHSS_Flyer.pdf</t>
@@ -691,7 +691,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov/assets/files/awardees/Sample_ContactingNSFSBIRCompanies.docx</t>
@@ -716,7 +716,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -724,7 +724,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/resources/awardees/supplement/</t>
@@ -771,7 +771,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov</t>
@@ -779,7 +779,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>/resources/awardees/instructions/</t>
@@ -846,7 +846,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="14"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://seedfund.nsf.gov/assets/files/awardees/ED-Supp-Template.docx</t>
@@ -1014,6 +1014,42 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://seedfund.nsf.gov/assets/files/awardees/phase-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> (separate phase 1 content on its own: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://seedfund.nsf.gov/assets/files/awardees/phase-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
@@ -1047,6 +1083,42 @@
   </si>
   <si>
     <t>https://www.nsf.gov/eng/iip/sbir/reporting2.jsp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://seedfund.nsf.gov/assets/files/awardees/phase-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">/reporting/ (separate phase 1 content on its own: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://seedfund.nsf.gov/assets/files/awardees/phase-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>/reporting/)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1174,7 +1246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1182,6 +1254,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -1200,16 +1277,27 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="14"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="14"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="15"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="15"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1222,8 +1310,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1235,9 +1329,7 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -1247,30 +1339,116 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="10"/>
-      </left>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
         <color indexed="11"/>
       </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -1282,42 +1460,66 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1336,10 +1538,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffb41700"/>
+      <rgbColor rgb="ffcc503e"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1356,10 +1561,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1536,11 +1741,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1549,7 +1757,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1564,12 +1772,12 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -1826,10 +2034,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2120,7 +2328,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -2401,703 +2609,767 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="69.1719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="82.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="82.25" style="1" customWidth="1"/>
-    <col min="4" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="82.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="82.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.35156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.35156" style="1" customWidth="1"/>
+    <col min="6" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" t="s" s="7">
         <v>3</v>
       </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="A3" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="11">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="A4" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="9">
+      <c r="B4" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+      <c r="A5" t="s" s="13">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="9">
+      <c r="B5" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="A6" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="9">
+      <c r="B6" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
+      <c r="A7" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="9">
+      <c r="B7" t="s" s="14">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="8">
+      <c r="A8" t="s" s="13">
         <v>13</v>
       </c>
-      <c r="B8" t="s" s="9">
+      <c r="B8" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="8">
+      <c r="A9" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="B9" t="s" s="9">
+      <c r="B9" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="8">
+      <c r="A10" t="s" s="13">
         <v>15</v>
       </c>
-      <c r="B10" t="s" s="9">
+      <c r="B10" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="8">
+      <c r="A11" t="s" s="13">
         <v>17</v>
       </c>
-      <c r="B11" t="s" s="9">
+      <c r="B11" t="s" s="14">
         <v>18</v>
       </c>
-      <c r="C11" t="s" s="9">
+      <c r="C11" t="s" s="14">
         <v>19</v>
       </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="8">
+      <c r="A12" t="s" s="13">
         <v>20</v>
       </c>
-      <c r="B12" t="s" s="9">
+      <c r="B12" t="s" s="14">
         <v>21</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="8">
+      <c r="A13" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="B13" t="s" s="9">
+      <c r="B13" t="s" s="14">
         <v>23</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="8">
+      <c r="A14" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="B14" t="s" s="9">
+      <c r="B14" t="s" s="14">
         <v>25</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="8">
+      <c r="A15" t="s" s="13">
         <v>26</v>
       </c>
-      <c r="B15" t="s" s="9">
+      <c r="B15" t="s" s="14">
         <v>27</v>
       </c>
-      <c r="C15" t="s" s="9">
+      <c r="C15" t="s" s="14">
         <v>28</v>
       </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="8">
+      <c r="A16" t="s" s="13">
         <v>29</v>
       </c>
-      <c r="B16" t="s" s="9">
+      <c r="B16" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="C16" t="s" s="9">
+      <c r="C16" t="s" s="14">
         <v>31</v>
       </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="8">
+      <c r="A17" t="s" s="13">
         <v>32</v>
       </c>
-      <c r="B17" t="s" s="9">
+      <c r="B17" t="s" s="14">
         <v>33</v>
       </c>
-      <c r="C17" t="s" s="9">
+      <c r="C17" t="s" s="14">
         <v>34</v>
       </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="8">
+      <c r="A18" t="s" s="13">
         <v>35</v>
       </c>
-      <c r="B18" t="s" s="9">
+      <c r="B18" t="s" s="14">
         <v>36</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="8">
+      <c r="A19" t="s" s="13">
         <v>37</v>
       </c>
-      <c r="B19" t="s" s="9">
+      <c r="B19" t="s" s="14">
         <v>38</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="8">
+      <c r="A20" t="s" s="13">
         <v>39</v>
       </c>
-      <c r="B20" t="s" s="9">
+      <c r="B20" t="s" s="14">
         <v>40</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="8">
+      <c r="A21" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="B21" t="s" s="9">
+      <c r="B21" t="s" s="14">
         <v>42</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="8">
+      <c r="A22" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="B22" t="s" s="9">
+      <c r="B22" t="s" s="14">
         <v>21</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="8">
+      <c r="A23" t="s" s="13">
         <v>44</v>
       </c>
-      <c r="B23" t="s" s="9">
+      <c r="B23" t="s" s="14">
         <v>45</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="8">
+      <c r="A24" t="s" s="13">
         <v>46</v>
       </c>
-      <c r="B24" t="s" s="9">
+      <c r="B24" t="s" s="14">
         <v>47</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="8">
+      <c r="A25" t="s" s="13">
         <v>48</v>
       </c>
-      <c r="B25" t="s" s="9">
+      <c r="B25" t="s" s="14">
         <v>49</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="8">
+      <c r="A26" t="s" s="13">
         <v>50</v>
       </c>
-      <c r="B26" t="s" s="9">
+      <c r="B26" t="s" s="14">
         <v>51</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="8">
+      <c r="A27" t="s" s="13">
         <v>52</v>
       </c>
-      <c r="B27" t="s" s="9">
+      <c r="B27" t="s" s="14">
         <v>53</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="8">
+      <c r="A28" t="s" s="13">
         <v>54</v>
       </c>
-      <c r="B28" t="s" s="9">
+      <c r="B28" t="s" s="14">
         <v>55</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="8">
+      <c r="A29" t="s" s="13">
         <v>56</v>
       </c>
-      <c r="B29" t="s" s="9">
+      <c r="B29" t="s" s="14">
         <v>57</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="8">
+      <c r="A30" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B30" t="s" s="9">
+      <c r="B30" t="s" s="14">
         <v>59</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" t="s" s="8">
+      <c r="A31" t="s" s="13">
         <v>60</v>
       </c>
-      <c r="B31" t="s" s="9">
+      <c r="B31" t="s" s="14">
         <v>61</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" t="s" s="8">
+      <c r="A32" t="s" s="13">
         <v>62</v>
       </c>
-      <c r="B32" t="s" s="9">
+      <c r="B32" t="s" s="14">
         <v>63</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" t="s" s="8">
+      <c r="A33" t="s" s="13">
         <v>64</v>
       </c>
-      <c r="B33" t="s" s="9">
+      <c r="B33" t="s" s="14">
         <v>65</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" t="s" s="8">
+      <c r="A34" t="s" s="13">
         <v>66</v>
       </c>
-      <c r="B34" t="s" s="9">
+      <c r="B34" t="s" s="14">
         <v>67</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" t="s" s="8">
+      <c r="A35" t="s" s="13">
         <v>68</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" t="s" s="9">
+      <c r="B35" s="15"/>
+      <c r="C35" t="s" s="14">
         <v>69</v>
       </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" t="s" s="8">
+      <c r="A36" t="s" s="13">
         <v>70</v>
       </c>
-      <c r="B36" t="s" s="9">
+      <c r="B36" t="s" s="14">
         <v>71</v>
       </c>
-      <c r="C36" t="s" s="9">
+      <c r="C36" t="s" s="14">
         <v>72</v>
       </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" t="s" s="8">
+      <c r="A37" t="s" s="13">
         <v>73</v>
       </c>
-      <c r="B37" t="s" s="9">
+      <c r="B37" t="s" s="14">
         <v>74</v>
       </c>
-      <c r="C37" t="s" s="9">
+      <c r="C37" t="s" s="14">
         <v>75</v>
       </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" t="s" s="8">
+      <c r="A38" t="s" s="13">
         <v>76</v>
       </c>
-      <c r="B38" t="s" s="9">
+      <c r="B38" t="s" s="14">
         <v>77</v>
       </c>
-      <c r="C38" t="s" s="9">
+      <c r="C38" t="s" s="14">
         <v>78</v>
       </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" t="s" s="8">
+      <c r="A39" t="s" s="13">
         <v>79</v>
       </c>
-      <c r="B39" t="s" s="9">
+      <c r="B39" t="s" s="14">
         <v>80</v>
       </c>
-      <c r="C39" t="s" s="9">
+      <c r="C39" t="s" s="14">
         <v>81</v>
       </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" t="s" s="8">
+      <c r="A40" t="s" s="13">
         <v>82</v>
       </c>
-      <c r="B40" t="s" s="9">
+      <c r="B40" t="s" s="14">
         <v>83</v>
       </c>
-      <c r="C40" t="s" s="9">
+      <c r="C40" t="s" s="14">
         <v>84</v>
       </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
     </row>
     <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" t="s" s="8">
+      <c r="A41" t="s" s="13">
         <v>85</v>
       </c>
-      <c r="B41" t="s" s="9">
+      <c r="B41" t="s" s="14">
         <v>86</v>
       </c>
-      <c r="C41" t="s" s="9">
+      <c r="C41" t="s" s="14">
         <v>87</v>
       </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" t="s" s="8">
+      <c r="A42" t="s" s="13">
         <v>88</v>
       </c>
-      <c r="B42" t="s" s="9">
+      <c r="B42" t="s" s="14">
         <v>89</v>
       </c>
-      <c r="C42" t="s" s="9">
+      <c r="C42" t="s" s="14">
         <v>90</v>
       </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" t="s" s="8">
+      <c r="A43" t="s" s="13">
         <v>91</v>
       </c>
-      <c r="B43" t="s" s="9">
+      <c r="B43" t="s" s="14">
         <v>92</v>
       </c>
-      <c r="C43" t="s" s="9">
+      <c r="C43" t="s" s="14">
         <v>93</v>
       </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" t="s" s="8">
+      <c r="A44" t="s" s="13">
         <v>94</v>
       </c>
-      <c r="B44" t="s" s="9">
+      <c r="B44" t="s" s="14">
         <v>95</v>
       </c>
-      <c r="C44" t="s" s="9">
+      <c r="C44" t="s" s="14">
         <v>96</v>
       </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" t="s" s="8">
+      <c r="A45" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" t="s" s="9">
+      <c r="B45" s="15"/>
+      <c r="C45" t="s" s="14">
         <v>98</v>
       </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" ht="32.05" customHeight="1">
-      <c r="A46" t="s" s="8">
+      <c r="A46" t="s" s="13">
         <v>99</v>
       </c>
-      <c r="B46" t="s" s="9">
+      <c r="B46" t="s" s="14">
         <v>100</v>
       </c>
-      <c r="C46" t="s" s="9">
+      <c r="C46" t="s" s="14">
         <v>101</v>
       </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" t="s" s="8">
+      <c r="A47" t="s" s="13">
         <v>102</v>
       </c>
-      <c r="B47" t="s" s="9">
+      <c r="B47" t="s" s="14">
         <v>103</v>
       </c>
-      <c r="C47" t="s" s="9">
+      <c r="C47" t="s" s="14">
         <v>104</v>
       </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" t="s" s="8">
+      <c r="A48" t="s" s="13">
         <v>105</v>
       </c>
-      <c r="B48" t="s" s="11">
+      <c r="B48" t="s" s="16">
         <v>106</v>
       </c>
-      <c r="C48" t="s" s="9">
+      <c r="C48" t="s" s="14">
         <v>107</v>
       </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" t="s" s="8">
+      <c r="A49" t="s" s="13">
         <v>108</v>
       </c>
-      <c r="B49" t="s" s="11">
+      <c r="B49" t="s" s="16">
         <v>109</v>
       </c>
-      <c r="C49" t="s" s="9">
+      <c r="C49" t="s" s="14">
         <v>110</v>
       </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" t="s" s="8">
+      <c r="A50" t="s" s="13">
         <v>111</v>
       </c>
-      <c r="B50" t="s" s="11">
+      <c r="B50" t="s" s="16">
         <v>112</v>
       </c>
-      <c r="C50" t="s" s="9">
+      <c r="C50" t="s" s="14">
         <v>113</v>
       </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" t="s" s="8">
+      <c r="A51" t="s" s="13">
         <v>114</v>
       </c>
-      <c r="B51" t="s" s="9">
+      <c r="B51" t="s" s="14">
         <v>115</v>
       </c>
-      <c r="C51" t="s" s="9">
+      <c r="C51" t="s" s="14">
         <v>116</v>
       </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" t="s" s="8">
+      <c r="A52" t="s" s="13">
         <v>117</v>
       </c>
-      <c r="B52" t="s" s="9">
+      <c r="B52" t="s" s="14">
         <v>118</v>
       </c>
-      <c r="C52" t="s" s="9">
+      <c r="C52" t="s" s="14">
         <v>119</v>
       </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" t="s" s="8">
+      <c r="A53" t="s" s="13">
         <v>120</v>
       </c>
-      <c r="B53" t="s" s="9">
+      <c r="B53" t="s" s="14">
         <v>121</v>
       </c>
-      <c r="C53" t="s" s="9">
+      <c r="C53" t="s" s="14">
         <v>122</v>
       </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" t="s" s="8">
+      <c r="A54" t="s" s="13">
         <v>111</v>
       </c>
-      <c r="B54" t="s" s="9">
+      <c r="B54" t="s" s="14">
         <v>112</v>
       </c>
-      <c r="C54" t="s" s="9">
+      <c r="C54" t="s" s="14">
         <v>113</v>
       </c>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" t="s" s="8">
+      <c r="A55" t="s" s="13">
         <v>123</v>
       </c>
-      <c r="B55" t="s" s="9">
+      <c r="B55" t="s" s="14">
         <v>124</v>
       </c>
-      <c r="C55" t="s" s="9">
+      <c r="C55" t="s" s="14">
         <v>125</v>
       </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="9"/>
     </row>
     <row r="56" ht="44.05" customHeight="1">
-      <c r="A56" t="s" s="8">
+      <c r="A56" t="s" s="13">
         <v>126</v>
       </c>
-      <c r="B56" s="10"/>
-      <c r="C56" t="s" s="9">
+      <c r="B56" t="s" s="17">
         <v>127</v>
       </c>
-    </row>
-    <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" t="s" s="8">
+      <c r="C56" t="s" s="14">
         <v>128</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" t="s" s="9">
+      <c r="D56" s="8"/>
+      <c r="E56" s="9"/>
+    </row>
+    <row r="57" ht="26.7" customHeight="1">
+      <c r="A57" t="s" s="13">
         <v>129</v>
       </c>
+      <c r="B57" t="s" s="17">
+        <v>130</v>
+      </c>
+      <c r="C57" t="s" s="14">
+        <v>131</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="9"/>
     </row>
     <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" t="s" s="8">
-        <v>130</v>
-      </c>
-      <c r="B58" t="s" s="9">
-        <v>131</v>
-      </c>
-      <c r="C58" t="s" s="9">
+      <c r="A58" t="s" s="13">
         <v>132</v>
       </c>
+      <c r="B58" t="s" s="14">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s" s="14">
+        <v>134</v>
+      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" t="s" s="8">
-        <v>133</v>
-      </c>
-      <c r="B59" t="s" s="9">
-        <v>134</v>
-      </c>
-      <c r="C59" t="s" s="9">
+      <c r="A59" t="s" s="13">
         <v>135</v>
       </c>
+      <c r="B59" t="s" s="14">
+        <v>136</v>
+      </c>
+      <c r="C59" t="s" s="14">
+        <v>137</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" t="s" s="8">
-        <v>136</v>
-      </c>
-      <c r="B60" t="s" s="9">
-        <v>137</v>
-      </c>
-      <c r="C60" t="s" s="9">
+      <c r="A60" t="s" s="13">
         <v>138</v>
       </c>
+      <c r="B60" t="s" s="14">
+        <v>139</v>
+      </c>
+      <c r="C60" t="s" s="14">
+        <v>140</v>
+      </c>
+      <c r="D60" s="8"/>
+      <c r="E60" s="9"/>
     </row>
     <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" t="s" s="8">
-        <v>139</v>
-      </c>
-      <c r="B61" t="s" s="9">
-        <v>140</v>
-      </c>
-      <c r="C61" t="s" s="9">
+      <c r="A61" t="s" s="13">
         <v>141</v>
       </c>
+      <c r="B61" t="s" s="14">
+        <v>142</v>
+      </c>
+      <c r="C61" t="s" s="14">
+        <v>143</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="9"/>
     </row>
     <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" t="s" s="8">
-        <v>142</v>
-      </c>
-      <c r="B62" t="s" s="9">
-        <v>143</v>
-      </c>
-      <c r="C62" s="10"/>
+      <c r="A62" t="s" s="13">
+        <v>144</v>
+      </c>
+      <c r="B62" t="s" s="14">
+        <v>145</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="B4" r:id="rId2" location="" tooltip="" display=""/>
-    <hyperlink ref="B5" r:id="rId3" location="" tooltip="" display=""/>
-    <hyperlink ref="B6" r:id="rId4" location="" tooltip="" display=""/>
-    <hyperlink ref="B7" r:id="rId5" location="" tooltip="" display=""/>
-    <hyperlink ref="B8" r:id="rId6" location="" tooltip="" display=""/>
-    <hyperlink ref="B9" r:id="rId7" location="" tooltip="" display=""/>
-    <hyperlink ref="B10" r:id="rId8" location="" tooltip="" display=""/>
-    <hyperlink ref="C11" r:id="rId9" location="" tooltip="" display=""/>
-    <hyperlink ref="B12" r:id="rId10" location="" tooltip="" display=""/>
-    <hyperlink ref="B13" r:id="rId11" location="" tooltip="" display=""/>
-    <hyperlink ref="B14" r:id="rId12" location="" tooltip="" display=""/>
-    <hyperlink ref="C15" r:id="rId13" location="" tooltip="" display=""/>
-    <hyperlink ref="C16" r:id="rId14" location="" tooltip="" display=""/>
-    <hyperlink ref="C17" r:id="rId15" location="" tooltip="" display=""/>
-    <hyperlink ref="B18" r:id="rId16" location="" tooltip="" display=""/>
-    <hyperlink ref="B19" r:id="rId17" location="" tooltip="" display=""/>
-    <hyperlink ref="B20" r:id="rId18" location="" tooltip="" display=""/>
-    <hyperlink ref="B21" r:id="rId19" location="" tooltip="" display=""/>
-    <hyperlink ref="B22" r:id="rId20" location="" tooltip="" display=""/>
-    <hyperlink ref="B23" r:id="rId21" location="" tooltip="" display=""/>
-    <hyperlink ref="B24" r:id="rId22" location="" tooltip="" display=""/>
-    <hyperlink ref="B25" r:id="rId23" location="" tooltip="" display=""/>
-    <hyperlink ref="B26" r:id="rId24" location="" tooltip="" display=""/>
-    <hyperlink ref="B27" r:id="rId25" location="" tooltip="" display=""/>
-    <hyperlink ref="B28" r:id="rId26" location="" tooltip="" display=""/>
-    <hyperlink ref="B29" r:id="rId27" location="" tooltip="" display=""/>
-    <hyperlink ref="B30" r:id="rId28" location="" tooltip="" display=""/>
-    <hyperlink ref="B31" r:id="rId29" location="" tooltip="" display=""/>
-    <hyperlink ref="B32" r:id="rId30" location="" tooltip="" display=""/>
-    <hyperlink ref="B33" r:id="rId31" location="" tooltip="" display=""/>
-    <hyperlink ref="B34" r:id="rId32" location="" tooltip="" display=""/>
-    <hyperlink ref="B36" r:id="rId33" location="" tooltip="" display=""/>
-    <hyperlink ref="C36" r:id="rId34" location="" tooltip="" display=""/>
-    <hyperlink ref="B37" r:id="rId35" location="" tooltip="" display=""/>
-    <hyperlink ref="C37" r:id="rId36" location="" tooltip="" display=""/>
-    <hyperlink ref="B38" r:id="rId37" location="" tooltip="" display=""/>
-    <hyperlink ref="C38" r:id="rId38" location="" tooltip="" display=""/>
-    <hyperlink ref="B39" r:id="rId39" location="" tooltip="" display=""/>
-    <hyperlink ref="C39" r:id="rId40" location="" tooltip="" display=""/>
-    <hyperlink ref="B40" r:id="rId41" location="" tooltip="" display=""/>
-    <hyperlink ref="C40" r:id="rId42" location="" tooltip="" display=""/>
-    <hyperlink ref="C41" r:id="rId43" location="" tooltip="" display=""/>
-    <hyperlink ref="C42" r:id="rId44" location="" tooltip="" display=""/>
-    <hyperlink ref="C43" r:id="rId45" location="" tooltip="" display=""/>
-    <hyperlink ref="B44" r:id="rId46" location="" tooltip="" display=""/>
-    <hyperlink ref="C44" r:id="rId47" location="" tooltip="" display=""/>
-    <hyperlink ref="C45" r:id="rId48" location="" tooltip="" display=""/>
-    <hyperlink ref="B46" r:id="rId49" location="" tooltip="" display=""/>
-    <hyperlink ref="C46" r:id="rId50" location="" tooltip="" display=""/>
-    <hyperlink ref="B47" r:id="rId51" location="" tooltip="" display=""/>
-    <hyperlink ref="C47" r:id="rId52" location="" tooltip="" display=""/>
-    <hyperlink ref="C48" r:id="rId53" location="" tooltip="" display=""/>
-    <hyperlink ref="C49" r:id="rId54" location="" tooltip="" display=""/>
-    <hyperlink ref="C50" r:id="rId55" location="" tooltip="" display=""/>
-    <hyperlink ref="C51" r:id="rId56" location="" tooltip="" display=""/>
-    <hyperlink ref="C52" r:id="rId57" location="" tooltip="" display=""/>
-    <hyperlink ref="C53" r:id="rId58" location="" tooltip="" display=""/>
-    <hyperlink ref="C54" r:id="rId59" location="" tooltip="" display=""/>
-    <hyperlink ref="B55" r:id="rId60" location="" tooltip="" display=""/>
-    <hyperlink ref="C55" r:id="rId61" location="" tooltip="" display=""/>
-    <hyperlink ref="C56" r:id="rId62" location="" tooltip="" display=""/>
-    <hyperlink ref="C57" r:id="rId63" location="" tooltip="" display=""/>
-    <hyperlink ref="C58" r:id="rId64" location="" tooltip="" display=""/>
-    <hyperlink ref="C59" r:id="rId65" location="" tooltip="" display=""/>
-    <hyperlink ref="C60" r:id="rId66" location="" tooltip="" display=""/>
-    <hyperlink ref="C61" r:id="rId67" location="" tooltip="" display=""/>
-    <hyperlink ref="B62" r:id="rId68" location="" tooltip="" display=""/>
+    <hyperlink ref="B56" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="B57" r:id="rId2" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
added phase 2b supplement URL
</commit_message>
<xml_diff>
--- a/assets/files/redirect.xlsx
+++ b/assets/files/redirect.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>Table 1</t>
   </si>
@@ -743,6 +743,9 @@
   </si>
   <si>
     <t>https://www.nsf.gov/eng/iip/sbir/Supplement/supplemental_phase-iib.jsp</t>
+  </si>
+  <si>
+    <t>https://seedfund.nsf.gov/resources/awardees/supplement/phase-2b</t>
   </si>
   <si>
     <r>
@@ -1509,10 +1512,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -3137,227 +3140,229 @@
       <c r="A45" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="B45" s="15"/>
+      <c r="B45" t="s" s="16">
+        <v>98</v>
+      </c>
       <c r="C45" t="s" s="14">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
     </row>
     <row r="46" ht="32.05" customHeight="1">
       <c r="A46" t="s" s="13">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s" s="14">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s" s="14">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="13">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s" s="14">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s" s="14">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="13">
-        <v>105</v>
-      </c>
-      <c r="B48" t="s" s="16">
         <v>106</v>
       </c>
+      <c r="B48" t="s" s="17">
+        <v>107</v>
+      </c>
       <c r="C48" t="s" s="14">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="13">
-        <v>108</v>
-      </c>
-      <c r="B49" t="s" s="16">
         <v>109</v>
       </c>
+      <c r="B49" t="s" s="17">
+        <v>110</v>
+      </c>
       <c r="C49" t="s" s="14">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="13">
-        <v>111</v>
-      </c>
-      <c r="B50" t="s" s="16">
         <v>112</v>
       </c>
+      <c r="B50" t="s" s="17">
+        <v>113</v>
+      </c>
       <c r="C50" t="s" s="14">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="13">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s" s="14">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C51" t="s" s="14">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="13">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s" s="14">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C52" t="s" s="14">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="13">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s" s="14">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s" s="14">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="13">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s" s="14">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C54" t="s" s="14">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="9"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="13">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B55" t="s" s="14">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C55" t="s" s="14">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
     </row>
     <row r="56" ht="44.05" customHeight="1">
       <c r="A56" t="s" s="13">
-        <v>126</v>
-      </c>
-      <c r="B56" t="s" s="17">
         <v>127</v>
       </c>
+      <c r="B56" t="s" s="16">
+        <v>128</v>
+      </c>
       <c r="C56" t="s" s="14">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="9"/>
     </row>
     <row r="57" ht="26.7" customHeight="1">
       <c r="A57" t="s" s="13">
-        <v>129</v>
-      </c>
-      <c r="B57" t="s" s="17">
         <v>130</v>
       </c>
+      <c r="B57" t="s" s="16">
+        <v>131</v>
+      </c>
       <c r="C57" t="s" s="14">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="13">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B58" t="s" s="14">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C58" t="s" s="14">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
     </row>
     <row r="59" ht="20.05" customHeight="1">
       <c r="A59" t="s" s="13">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s" s="14">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C59" t="s" s="14">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
     </row>
     <row r="60" ht="20.05" customHeight="1">
       <c r="A60" t="s" s="13">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B60" t="s" s="14">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s" s="14">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
     </row>
     <row r="61" ht="20.05" customHeight="1">
       <c r="A61" t="s" s="13">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s" s="14">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s" s="14">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
     </row>
     <row r="62" ht="20.05" customHeight="1">
       <c r="A62" t="s" s="13">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B62" t="s" s="14">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="18"/>

</xml_diff>